<commit_message>
all versions of CLEANED
</commit_message>
<xml_diff>
--- a/20200606 -CLEANED versions results-EM.xlsx
+++ b/20200606 -CLEANED versions results-EM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="6"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="T23 overview" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -409,10 +409,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -427,6 +424,9 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -15348,8 +15348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15541,8 +15541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:S17"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15600,13 +15600,13 @@
       <c r="L3" t="s">
         <v>73</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -15620,42 +15620,42 @@
         <f>[3]Productivity!$B$20</f>
         <v>5581.2456926987752</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <f>[4]Productivity!$B$20</f>
         <v>5668.9624998061408</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <f>[5]Productivity!$B$20</f>
         <v>5668.9624998061408</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="20">
         <f>[6]Productivity!$B$20</f>
         <v>5846.3799752288633</v>
       </c>
       <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <f>[2]SUMMARY!$G$9</f>
         <v>5017.2204013914588</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <f>[3]SUMMARY!$G$9</f>
         <v>1752.7770823509265</v>
       </c>
-      <c r="J4" s="21">
+      <c r="J4" s="20">
         <f>[4]SUMMARY!$G$9</f>
         <v>1905.0595313236815</v>
       </c>
-      <c r="K4" s="21">
+      <c r="K4" s="20">
         <f>[5]SUMMARY!$G$9</f>
         <v>1905.0595313236815</v>
       </c>
-      <c r="L4" s="21">
+      <c r="L4" s="20">
         <f>[6]SUMMARY!$G$9</f>
         <v>1716.6911582187438</v>
       </c>
-      <c r="M4" s="21"/>
+      <c r="M4" s="20"/>
       <c r="O4" t="s">
         <v>65</v>
       </c>
@@ -15739,7 +15739,7 @@
         <f>[5]SUMMARY!$D$40</f>
         <v>1490.6677199999999</v>
       </c>
-      <c r="S5" s="20">
+      <c r="S5" s="19">
         <f>[6]SUMMARY!$D$40</f>
         <v>1413.9834000000001</v>
       </c>
@@ -16244,7 +16244,7 @@
       <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <f>[2]SUMMARY!$G$27</f>
         <v>1021.7414929542122</v>
       </c>
@@ -16273,7 +16273,7 @@
         <f>[2]SUMMARY!$J$31</f>
         <v>3.4173297937601692</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <f>[3]SUMMARY!$J$31</f>
         <v>9.5978671768734696</v>
       </c>
@@ -16298,7 +16298,7 @@
         <f>[2]SUMMARY!$J$29</f>
         <v>0.2036469222422132</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>[3]SUMMARY!$J$29</f>
         <v>0.56507236620648416</v>
       </c>
@@ -16323,7 +16323,7 @@
         <f>[2]SUMMARY!$J$30</f>
         <v>2.3436276605122606</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <f>[3]SUMMARY!$J$30</f>
         <v>6.7163547169478264</v>
       </c>
@@ -16350,7 +16350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
@@ -16364,431 +16364,431 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="26">
         <f>'[2]GHG emissions'!$C$35</f>
         <v>8.4546269436760362</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="26">
         <f>'[3]GHG emissions'!$C$33</f>
         <v>3.2705423367870146</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="26">
         <f>'[4]GHG emissions'!$C$33</f>
         <v>3.5546892494377635</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="26">
         <f>'[5]GHG emissions'!$C$33</f>
         <v>5.4064343468192959</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="26">
         <f>'[6]GHG emissions'!$C$33</f>
         <v>3.4122400318547319</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="26">
         <f>'[2]GHG emissions'!$C$32</f>
         <v>1.6863661251003164</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="26">
         <f>'[3]GHG emissions'!$C$30</f>
         <v>0.71341817579003786</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="26">
         <f>'[4]GHG emissions'!$C$30</f>
         <v>0.76741540740446124</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="26">
         <f>'[5]GHG emissions'!$C$30</f>
         <v>0.55360197581303994</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <f>'[6]GHG emissions'!$C$30</f>
         <v>0.44208770298385219</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <f>'[2]GHG emissions'!$C$34</f>
         <v>2.3889138532971166</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="26">
         <f>'[3]GHG emissions'!$C$32</f>
         <v>0.74017266787624547</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="26">
         <f>'[4]GHG emissions'!$C$32</f>
         <v>0.80447936589383473</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <f>'[5]GHG emissions'!$C$32</f>
         <v>0.57641170552965204</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <f>'[6]GHG emissions'!$C$32</f>
         <v>0.63057762153211983</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <f>'[2]GHG emissions'!$C$38</f>
         <v>5.875355399441738E-3</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="26">
         <f>'[3]GHG emissions'!$C$36</f>
         <v>2.1323718724068162E-3</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="26">
         <f>'[4]GHG emissions'!$C$36</f>
         <v>2.3176337714357511E-3</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="26">
         <f>'[5]GHG emissions'!$C$36</f>
         <v>2.9128375527369577E-2</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="26">
         <f>'[6]GHG emissions'!$C$36</f>
         <v>2.224757828078044E-3</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <f>SUM(C4:C7)</f>
         <v>12.535782277472912</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <f>SUM(D4:D7)</f>
         <v>4.7262655523257049</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <f t="shared" ref="E8:G8" si="0">SUM(E4:E7)</f>
         <v>5.1289016565074954</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <f t="shared" si="0"/>
         <v>6.5655764036893567</v>
       </c>
-      <c r="G8" s="30">
+      <c r="G8" s="29">
         <f t="shared" si="0"/>
         <v>4.4871301141987816</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="26">
         <f>'[2]GHG emissions'!$D$35</f>
         <v>5.4169933237552588</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="26">
         <f>'[3]GHG emissions'!$D$33</f>
         <v>5.0126127052395244</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="26">
         <f>'[4]GHG emissions'!$D$33</f>
         <v>5.5337362896641116</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="26">
         <f>'[5]GHG emissions'!$D$33</f>
         <v>5.5337362896641116</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="26">
         <f>'[6]GHG emissions'!$D$33</f>
         <v>2.918314478757952</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="26">
         <f>'[2]GHG emissions'!$D$32</f>
         <v>0.46875414155080991</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="26">
         <f>'[3]GHG emissions'!$D$30</f>
         <v>0.36171343898979047</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="26">
         <f>'[4]GHG emissions'!$D$30</f>
         <v>9.0716494235919098E-2</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="26">
         <f>'[5]GHG emissions'!$D$30</f>
         <v>0.39604178314834426</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="26">
         <f>'[6]GHG emissions'!$D$30</f>
         <v>9.0292697668769184E-2</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="26">
         <f>'[2]GHG emissions'!$D$34</f>
         <v>3.2442631089350753</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="26">
         <f>'[3]GHG emissions'!$D$32</f>
         <v>1.0967281237811013</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="26">
         <f>'[4]GHG emissions'!$D$32</f>
         <v>0.38258252863613396</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="26">
         <f>'[5]GHG emissions'!$D$32</f>
         <v>1.2306473465388386</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="26">
         <f>'[6]GHG emissions'!$D$32</f>
         <v>0.43373379317942351</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="26">
         <f>'[2]GHG emissions'!$D$38</f>
         <v>5.875355399441738E-3</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="26">
         <f>'[3]GHG emissions'!$D$36</f>
         <v>2.1323718724068162E-3</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="26">
         <f>'[4]GHG emissions'!$D$36</f>
         <v>2.3176337714357511E-3</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="26">
         <f>'[5]GHG emissions'!$D$36</f>
         <v>2.9128375527369577E-2</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="26">
         <f>'[6]GHG emissions'!$D$36</f>
         <v>2.224757828078044E-3</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <f>SUM(C11:C14)</f>
         <v>9.135885929640585</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <f>SUM(D11:D14)</f>
         <v>6.4731866398828233</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E15" s="29">
         <f t="shared" ref="E15:G15" si="1">SUM(E11:E14)</f>
         <v>6.009352946307601</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="29">
         <f t="shared" si="1"/>
         <v>7.1895537948786634</v>
       </c>
-      <c r="G15" s="30">
+      <c r="G15" s="29">
         <f t="shared" si="1"/>
         <v>3.444565727434223</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="25">
+      <c r="C18" s="24">
         <f>[2]SUMMARY!$G$24</f>
         <v>9.1300105742411439</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="25">
         <f>[3]SUMMARY!$G$24</f>
         <v>6.4710542680104162</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="25">
         <f>[4]SUMMARY!$G$24</f>
         <v>6.0070353125361651</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="25">
         <f>[5]SUMMARY!$G$24</f>
         <v>7.1604254193512942</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="25">
         <f>[6]SUMMARY!$G$24</f>
         <v>3.4423409696061444</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="22" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="26">
         <f>[2]SUMMARY!$J$26</f>
         <v>30.53635128635991</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="26">
         <f>[3]SUMMARY!$J$26</f>
         <v>62.707432859582482</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="26">
         <f>[4]SUMMARY!$J$26</f>
         <v>53.557747015674977</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="26">
         <f>[5]SUMMARY!$J$26</f>
         <v>63.841185074091605</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="26">
         <f>[6]SUMMARY!$J$26</f>
         <v>36.259249364043768</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="26">
         <f>[2]SUMMARY!$J$25</f>
         <v>20.942034232840793</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="26">
         <f>[3]SUMMARY!$J$25</f>
         <v>43.881140956916397</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="26">
         <f>[4]SUMMARY!$J$25</f>
         <v>37.478412669074295</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="26">
         <f>[5]SUMMARY!$J$25</f>
         <v>44.674513264892937</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="26">
         <f>[6]SUMMARY!$J$25</f>
         <v>22.373656008999884</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="26">
         <f>[2]SUMMARY!$J$24</f>
         <v>1.8197348021045792</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="26">
         <f>[3]SUMMARY!$J$24</f>
         <v>3.6918866256118901</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="26">
         <f>[4]SUMMARY!$J$24</f>
         <v>3.1532008390112258</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="26">
         <f>[5]SUMMARY!$J$24</f>
         <v>3.7586360434500734</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="26">
         <f>[6]SUMMARY!$J$24</f>
         <v>2.0052185584610061</v>
       </c>

</xml_diff>